<commit_message>
More 8 Start 9
</commit_message>
<xml_diff>
--- a/Protokoll 8/Versuch 6 Berechnungen.xlsx
+++ b/Protokoll 8/Versuch 6 Berechnungen.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="220" yWindow="0" windowWidth="25600" windowHeight="15520" tabRatio="500"/>
+    <workbookView xWindow="6360" yWindow="0" windowWidth="22500" windowHeight="13720" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -167,8 +167,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="151">
+  <cellStyleXfs count="161">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -324,7 +334,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="151">
+  <cellStyles count="161">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -400,6 +410,11 @@
     <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -475,6 +490,11 @@
     <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -806,8 +826,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:R47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="L48" sqref="L48"/>
+    <sheetView tabSelected="1" topLeftCell="F43" workbookViewId="0">
+      <selection activeCell="M43" sqref="M43:M47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1208,8 +1228,8 @@
     </row>
     <row r="17" spans="1:18">
       <c r="B17">
-        <f>B16+0.14994</f>
-        <v>0.44955000000000001</v>
+        <f>B16+0.04994</f>
+        <v>0.34954999999999997</v>
       </c>
       <c r="C17">
         <v>0.7</v>
@@ -1373,8 +1393,8 @@
     </row>
     <row r="20" spans="1:18">
       <c r="B20">
-        <f>B19+0.14994</f>
-        <v>0.54958000000000007</v>
+        <f>B19+0.04994</f>
+        <v>0.44958000000000004</v>
       </c>
       <c r="C20">
         <v>0.89</v>
@@ -1802,7 +1822,7 @@
         <v>16</v>
       </c>
       <c r="C43">
-        <v>2.0349499999999998</v>
+        <v>2.0329999999999999</v>
       </c>
       <c r="D43">
         <v>9.91</v>
@@ -1815,7 +1835,7 @@
       </c>
       <c r="G43">
         <f>(9.81*F43^3)/(4*E43^3*D43*C43)</f>
-        <v>212895.12280704806</v>
+        <v>213099.32619586936</v>
       </c>
       <c r="I43">
         <v>8.0000000000000002E-3</v>
@@ -1830,12 +1850,12 @@
         <v>1</v>
       </c>
       <c r="M43">
-        <f>SQRT((I43/C43)^2+(J43/D43)^2+(K43/E43)^2+(L43/F43)^2)</f>
-        <v>4.3168790111785373E-3</v>
+        <f>SQRT((I43/C43)^2+(J43/D43)^2+(3*K43/E43)^2+(3*L43/F43)^2)</f>
+        <v>6.3337309326923514E-3</v>
       </c>
       <c r="N43">
         <f>G43*M43</f>
-        <v>919.04248722802288</v>
+        <v>1349.7137940626753</v>
       </c>
     </row>
     <row r="44" spans="1:14">
@@ -1871,12 +1891,12 @@
         <v>1</v>
       </c>
       <c r="M44">
-        <f t="shared" ref="M44" si="12">SQRT((I44/C44)^2+(J44/D44)^2+(K44/E44)^2+(L44/F44)^2)</f>
-        <v>4.1684292998470287E-3</v>
+        <f t="shared" ref="M44:M47" si="12">SQRT((I44/C44)^2+(J44/D44)^2+(3*K44/E44)^2+(3*L44/F44)^2)</f>
+        <v>7.6563035364855562E-3</v>
       </c>
       <c r="N44">
         <f t="shared" ref="N44" si="13">G44*M44</f>
-        <v>284.57977491753036</v>
+        <v>522.69787499893766</v>
       </c>
     </row>
     <row r="45" spans="1:14">
@@ -1896,7 +1916,7 @@
         <v>608</v>
       </c>
       <c r="G45">
-        <f t="shared" ref="G44:G47" si="14">(9.81*F45^3)/(4*E45^3*D45*C45)</f>
+        <f t="shared" ref="G45:G46" si="14">(9.81*F45^3)/(4*E45^3*D45*C45)</f>
         <v>103509.3361635741</v>
       </c>
       <c r="I45">
@@ -1912,12 +1932,12 @@
         <v>1</v>
       </c>
       <c r="M45">
-        <f>SQRT((I45/C45)^2+(J45/D45)^2+(K45/E45)^2+(L45/F45)^2)</f>
-        <v>7.6946363744444607E-2</v>
+        <f t="shared" si="12"/>
+        <v>7.7123942282862415E-2</v>
       </c>
       <c r="N45">
         <f>G45*M45</f>
-        <v>7964.6670313883669</v>
+        <v>7983.0480680168921</v>
       </c>
     </row>
     <row r="46" spans="1:14">
@@ -1953,12 +1973,12 @@
         <v>1</v>
       </c>
       <c r="M46">
-        <f>SQRT((I46/C46)^2+(J46/D46)^2+(K46/E46)^2+(L46/F46)^2)</f>
-        <v>6.0300033440863314E-3</v>
+        <f t="shared" si="12"/>
+        <v>7.7011477222655791E-3</v>
       </c>
       <c r="N46">
         <f>G46*M46</f>
-        <v>552.36472762724554</v>
+        <v>705.4461036407522</v>
       </c>
     </row>
     <row r="47" spans="1:14">
@@ -1994,17 +2014,20 @@
         <v>1</v>
       </c>
       <c r="M47">
-        <f>SQRT((I47/C47)^2+(J47/D47)^2+(K47/E47)^2+(L47/F47)^2)</f>
-        <v>1.5774502552279891E-2</v>
+        <f t="shared" si="12"/>
+        <v>1.6777523767696777E-2</v>
       </c>
       <c r="N47">
         <f>G47*M47</f>
-        <v>1090.6605890657108</v>
+        <v>1160.0102060204388</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <ignoredErrors>
+    <ignoredError sqref="E15:E23" formulaRange="1"/>
+  </ignoredErrors>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>